<commit_message>
Updating rmd files and linking them to html's.
</commit_message>
<xml_diff>
--- a/prep/food_provision/Fisheries/raw/ices_bmsy.xlsx
+++ b/prep/food_provision/Fisheries/raw/ices_bmsy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaespinasse/github/nor-prep/prep/food_provision/Fisheries/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaespinasse/github/nor-prep/prep/food_provision/Fisheries/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E1B7EC-708B-E44E-8BBB-C5EF26696FD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD995799-D68F-0944-AF65-0C9F1E389FC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="7900" windowWidth="33540" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="8360" windowWidth="33540" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSB and Bmsy data" sheetId="1" r:id="rId1"/>
@@ -448,8 +448,8 @@
   <dimension ref="A1:N80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <pane ySplit="8" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>